<commit_message>
first GBP working version
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/GBP_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/GBP_MainChecks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="60" windowWidth="14550" windowHeight="8445"/>
+    <workbookView xWindow="20325" yWindow="-15" windowWidth="10215" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="MainChecks" sheetId="2" r:id="rId1"/>
@@ -16,11 +16,11 @@
     <definedName name="AllTriggers">MainChecks!$I$5:$I$5</definedName>
     <definedName name="Currency">MainChecks!$B$1</definedName>
     <definedName name="EvaluationDate">MainChecks!$C$3</definedName>
-    <definedName name="FirstIndex">MainChecks!$B$10</definedName>
+    <definedName name="FirstIndex">MainChecks!$B$11</definedName>
     <definedName name="InterestRatesTrigger">MainChecks!$I$5</definedName>
-    <definedName name="SecondIMMDate">MainChecks!$C$11</definedName>
+    <definedName name="SecondIMMDate">MainChecks!$C$12</definedName>
     <definedName name="Trigger">MainChecks!$I$2</definedName>
-    <definedName name="Yesterday">MainChecks!$C$8</definedName>
+    <definedName name="Yesterday">MainChecks!$C$9</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -186,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -561,6 +561,30 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -578,7 +602,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -667,9 +691,6 @@
     <xf numFmtId="167" fontId="8" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="167" fontId="6" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
@@ -693,6 +714,18 @@
     </xf>
     <xf numFmtId="4" fontId="7" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="8" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="6" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -788,9 +821,9 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Paused at 15:02:18</v>
+        <v>Updated at 18:28:49</v>
         <stp/>
-        <stp>{02CCA5F9-6041-493D-923A-5CD6D4D04C51}</stp>
+        <stp>{346E5213-D98C-4DA8-99C2-EAACB8469A7B}</stp>
         <tr r="I3" s="2"/>
       </tp>
     </main>
@@ -932,7 +965,7 @@
       <sheetData sheetId="0">
         <row r="27">
           <cell r="D27">
-            <v>27</v>
+            <v>42</v>
           </cell>
         </row>
       </sheetData>
@@ -1368,7 +1401,7 @@
   <dimension ref="A1:W59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1421,7 +1454,7 @@
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="9"/>
@@ -1436,7 +1469,7 @@
         <v>3</v>
       </c>
       <c r="I2" s="40">
-        <v>41768.625150462962</v>
+        <v>41771.761736111112</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="5"/>
@@ -1459,26 +1492,26 @@
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>GBPSTD</v>
       </c>
-      <c r="C3" s="49">
+      <c r="C3" s="48">
         <f>_xll.qlSettingsEvaluationDate(ISERROR(Trigger))</f>
-        <v>41768</v>
+        <v>41771</v>
       </c>
       <c r="D3" s="17"/>
-      <c r="E3" s="18" t="e">
+      <c r="E3" s="18">
         <f>_xll.qlYieldTSDiscount(B3,C3,,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="F3" s="19" t="str">
-        <f ca="1">IF(ISERROR(C3),_xll.ohRangeRetrieveError(C3),_xll.ohRangeRetrieveError(E3))</f>
-        <v>qlYieldTSDiscount - empty Handle cannot be dereferenced</v>
+        <f>IF(ISERROR(C3),_xll.ohRangeRetrieveError(C3),_xll.ohRangeRetrieveError(E3))</f>
+        <v/>
       </c>
       <c r="G3" s="12"/>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="46" t="str">
+      <c r="I3" s="45" t="str">
         <f>_xll.RData(H4,"LAST",,"FRQ:1S",,I4)</f>
-        <v>Paused at 15:02:18</v>
+        <v>Updated at 18:28:49</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="5"/>
@@ -1503,7 +1536,7 @@
       </c>
       <c r="C4" s="41">
         <f>EvaluationDate</f>
-        <v>41768</v>
+        <v>41771</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18">
@@ -1515,11 +1548,11 @@
         <v/>
       </c>
       <c r="G4" s="12"/>
-      <c r="H4" s="48" t="s">
+      <c r="H4" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="45">
-        <v>124.9375</v>
+      <c r="I4" s="44">
+        <v>124.78125</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="5"/>
@@ -1544,16 +1577,16 @@
       </c>
       <c r="C5" s="41">
         <f>EvaluationDate</f>
-        <v>41768</v>
+        <v>41771</v>
       </c>
       <c r="D5" s="17"/>
-      <c r="E5" s="18" t="e">
+      <c r="E5" s="18">
         <f>_xll.qlYieldTSDiscount(B5,C5,,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="F5" s="19" t="str">
-        <f ca="1">IF(ISERROR(C5),_xll.ohRangeRetrieveError(C5),_xll.ohRangeRetrieveError(E5))</f>
-        <v>qlYieldTSDiscount - empty Handle cannot be dereferenced</v>
+        <f>IF(ISERROR(C5),_xll.ohRangeRetrieveError(C5),_xll.ohRangeRetrieveError(E5))</f>
+        <v/>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="20" t="s">
@@ -1561,7 +1594,7 @@
       </c>
       <c r="I5" s="21">
         <f>[1]!TriggerCounter</f>
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="5"/>
@@ -1586,16 +1619,16 @@
       </c>
       <c r="C6" s="41">
         <f>EvaluationDate</f>
-        <v>41768</v>
+        <v>41771</v>
       </c>
       <c r="D6" s="17"/>
-      <c r="E6" s="18" t="e">
+      <c r="E6" s="18">
         <f>_xll.qlYieldTSDiscount(B6,C6,,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="F6" s="19" t="str">
-        <f ca="1">IF(ISERROR(C6),_xll.ohRangeRetrieveError(C6),_xll.ohRangeRetrieveError(E6))</f>
-        <v>qlYieldTSDiscount - empty Handle cannot be dereferenced</v>
+        <f>IF(ISERROR(C6),_xll.ohRangeRetrieveError(C6),_xll.ohRangeRetrieveError(E6))</f>
+        <v/>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="20" t="s">
@@ -1603,7 +1636,7 @@
       </c>
       <c r="I6" s="21">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>862</v>
+        <v>1383</v>
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="5"/>
@@ -1628,16 +1661,16 @@
       </c>
       <c r="C7" s="41">
         <f>EvaluationDate</f>
-        <v>41768</v>
+        <v>41771</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="18" t="e">
+      <c r="E7" s="18">
         <f>_xll.qlYieldTSDiscount(B7,C7,,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="F7" s="19" t="str">
-        <f ca="1">IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(E7))</f>
-        <v>qlYieldTSDiscount - empty Handle cannot be dereferenced</v>
+        <f>IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(E7))</f>
+        <v/>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="34" t="s">
@@ -1661,21 +1694,24 @@
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="42">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
-        <v>41766</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="26" t="e">
-        <f>_xll.qlIndexFixing(FirstIndex,C8)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F8" s="15" t="str">
-        <f ca="1">IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
-        <v>qlIndexFixing - Missing GBPLibor3M Actual/365 (Fixed) fixing for May 7th, 2014</v>
+      <c r="B8" s="27" t="str">
+        <f>UPPER(Currency)&amp;"1Y"</f>
+        <v>GBP1Y</v>
+      </c>
+      <c r="C8" s="55">
+        <f>EvaluationDate</f>
+        <v>41771</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="18">
+        <f>_xll.qlYieldTSDiscount(B8,C8,,Trigger)</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="19" t="str">
+        <f>IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
+        <v/>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="20" t="s">
@@ -1702,19 +1738,19 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="43">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
+      <c r="B9" s="24"/>
+      <c r="C9" s="54">
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
         <v>41767</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="29" t="e">
+      <c r="D9" s="25"/>
+      <c r="E9" s="26" t="e">
         <f>_xll.qlIndexFixing(FirstIndex,C9)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F9" s="19" t="str">
+      <c r="F9" s="15" t="str">
         <f ca="1">IF(ISERROR(C9),_xll.ohRangeRetrieveError(C9),_xll.ohRangeRetrieveError(E9))</f>
-        <v>qlIndexFixing - Missing GBPLibor3M Actual/365 (Fixed) fixing for May 8th, 2014</v>
+        <v/>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="22" t="s">
@@ -1741,15 +1777,12 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
-      <c r="B10" s="27" t="str">
-        <f>PROPER(Currency)&amp;IF(UPPER(Currency)="EUR","",IF(UPPER(Currency)="HKD","H","L"))&amp;"ibor3M"</f>
-        <v>GbpLibor3M</v>
-      </c>
-      <c r="C10" s="43">
-        <f>EvaluationDate</f>
+      <c r="B10" s="27"/>
+      <c r="C10" s="42">
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
         <v>41768</v>
       </c>
-      <c r="D10" s="28"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="29">
         <f>_xll.qlIndexFixing(FirstIndex,C10)</f>
         <v>5.2813000000000001E-3</v>
@@ -1783,19 +1816,22 @@
     </row>
     <row r="11" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="44">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlIMMNextDate(_xll.qlIMMNextDate(EvaluationDate+1)+1),-_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>41899</v>
-      </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32" t="e">
-        <f>_xll.qlIndexFixing(FirstIndex,C11,TRUE)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F11" s="33" t="str">
-        <f ca="1">IF(ISERROR(C11),_xll.ohRangeRetrieveError(C11),_xll.ohRangeRetrieveError(E11))</f>
-        <v>qlIndexFixing - null term structure set to this instance of GBPLibor3M Actual/365 (Fixed)</v>
+      <c r="B11" s="27" t="str">
+        <f>PROPER(Currency)&amp;IF(UPPER(Currency)="EUR","",IF(UPPER(Currency)="HKD","H","L"))&amp;"ibor3M"</f>
+        <v>GbpLibor3M</v>
+      </c>
+      <c r="C11" s="42">
+        <f>EvaluationDate</f>
+        <v>41771</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29">
+        <f>_xll.qlIndexFixing(FirstIndex,C11)</f>
+        <v>5.2810000006973277E-3</v>
+      </c>
+      <c r="F11" s="19" t="str">
+        <f>IF(ISERROR(C11),_xll.ohRangeRetrieveError(C11),_xll.ohRangeRetrieveError(E11))</f>
+        <v/>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="34" t="s">
@@ -1821,16 +1857,25 @@
       <c r="W11" s="5"/>
     </row>
     <row r="12" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="43">
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlIMMNextDate(_xll.qlIMMNextDate(EvaluationDate+1)+1),-_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
+        <v>41899</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32">
+        <f>_xll.qlIndexFixing(FirstIndex,C12,TRUE)</f>
+        <v>7.3601491837369916E-3</v>
+      </c>
+      <c r="F12" s="33" t="str">
+        <f>IF(ISERROR(C12),_xll.ohRangeRetrieveError(C12),_xll.ohRangeRetrieveError(E12))</f>
+        <v/>
+      </c>
+      <c r="G12" s="51"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="14"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -1845,17 +1890,17 @@
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
+    <row r="13" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="39"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -2872,6 +2917,11 @@
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>

</xml_diff>

<commit_message>
GBP Market Data Checks Modification
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/GBP_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/GBP_MainChecks.xlsx
@@ -276,6 +276,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -582,7 +583,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -710,6 +711,9 @@
     <xf numFmtId="172" fontId="6" fillId="0" borderId="8" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="1"/>
@@ -806,28 +810,34 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 17:31:15</v>
+        <v>Updated at 11:26:11</v>
         <stp/>
-        <stp>{2B911FD7-C0F1-4FEA-A7B9-7C651CD09A4C}</stp>
+        <stp>{4C473E17-AB62-4D1E-A30E-FEEB42EFAF5F}</stp>
+        <tr r="Q6" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 11:22:03</v>
+        <stp/>
+        <stp>{E2282FA0-CD62-4B95-A250-73EDB77D9EFC}</stp>
+        <tr r="Q7" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 11:26:57</v>
+        <stp/>
+        <stp>{DFAF9D8F-904D-46C0-9ED9-350D957991D8}</stp>
+        <tr r="P5" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 11:24:00</v>
+        <stp/>
+        <stp>{6E9F85D6-AAEC-43B6-98F0-E929F336C91D}</stp>
         <tr r="Q5" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 17:30:52</v>
+        <v>Updated at 11:26:34</v>
         <stp/>
-        <stp>{BE2EFEB2-3D36-49A6-8B66-358CFDE06EB5}</stp>
+        <stp>{0B383ECD-58AA-4CC9-9CBA-60D0C3D0D148}</stp>
         <tr r="P7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 17:30:47</v>
-        <stp/>
-        <stp>{170EB86B-BB30-4FCD-9EE5-8DDCA9213CE7}</stp>
-        <tr r="Q6" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 17:30:52</v>
-        <stp/>
-        <stp>{D9938D73-0AF6-4E5D-8D5B-9F8E61C00761}</stp>
-        <tr r="Q7" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1239,8 +1249,8 @@
     <col min="10" max="10" width="2.7109375" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="7" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="16" max="16" width="20.28515625" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="17" max="17" width="20.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="2" style="2" bestFit="1" customWidth="1"/>
@@ -1474,15 +1484,23 @@
       <c r="L5" s="27">
         <v>42002</v>
       </c>
-      <c r="M5" s="28">
-        <v>114.59</v>
-      </c>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
+      <c r="M5" s="59" t="str">
+        <f>N5&amp;"/"&amp;O5</f>
+        <v>118.79/118.81</v>
+      </c>
+      <c r="N5" s="28">
+        <v>118.79</v>
+      </c>
+      <c r="O5" s="28">
+        <v>118.81</v>
+      </c>
+      <c r="P5" s="28" t="str">
+        <f>_xll.RData(K5,{"BID","ASK"},,"FRQ:1S",,N5)</f>
+        <v>Updated at 11:26:57</v>
+      </c>
       <c r="Q5" s="29" t="str">
-        <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 17:31:15</v>
+        <f>_xll.RData(K5,"EXPIR_DATE",,"FRQ:1S",,L5)</f>
+        <v>Updated at 11:24:00</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>13</v>
@@ -1491,9 +1509,9 @@
       <c r="T5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="U5" s="11" t="e">
-        <f ca="1">_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
-        <v>#NAME?</v>
+      <c r="U5" s="11" t="str">
+        <f>_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
+        <v>1_52 / 1.5.0 / 1.5</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1545,14 +1563,14 @@
         <v>42172</v>
       </c>
       <c r="M6" s="30">
-        <v>99.070000000000007</v>
+        <v>99.32</v>
       </c>
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
       <c r="Q6" s="31" t="str">
         <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>Updated at 17:30:47</v>
+        <v>Updated at 11:26:11</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>13</v>
@@ -1561,9 +1579,9 @@
       <c r="T6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="U6" s="11" t="e">
-        <f ca="1">_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>#NAME?</v>
+      <c r="U6" s="11">
+        <f>_xll.ohRepositoryObjectCount(Trigger)</f>
+        <v>1599</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1613,25 +1631,25 @@
         <v>GBPSB6L10Y</v>
       </c>
       <c r="L7" s="24">
-        <v>41919</v>
+        <v>41983</v>
       </c>
       <c r="M7" s="33" t="str">
         <f>N7&amp;"/"&amp;O7</f>
-        <v>2.327/2.377</v>
+        <v>1.977/2.027</v>
       </c>
       <c r="N7" s="30">
-        <v>2.3270000000000004</v>
+        <v>1.9769999999999999</v>
       </c>
       <c r="O7" s="30">
-        <v>2.3770000000000002</v>
+        <v>2.0270000000000001</v>
       </c>
       <c r="P7" s="30" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Updated at 17:30:52</v>
+        <v>Updated at 11:26:34</v>
       </c>
       <c r="Q7" s="31" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Updated at 17:30:52</v>
+        <v>Updated at 11:22:03</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>13</v>
@@ -1808,20 +1826,20 @@
         <f>PROPER(Currency)&amp;VLOOKUP(Currency,FuturesTable,8,0)&amp;VLOOKUP(Currency,FuturesTable,2,0)</f>
         <v>GbpLibor6M</v>
       </c>
-      <c r="L10" s="22" t="e">
-        <f ca="1">_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M10" s="32" t="e">
-        <f ca="1">_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>#NAME?</v>
+      <c r="L10" s="22">
+        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>41982</v>
+      </c>
+      <c r="M10" s="32">
+        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>6.7843999999999995E-3</v>
       </c>
       <c r="N10" s="32"/>
       <c r="O10" s="32"/>
       <c r="P10" s="32"/>
-      <c r="Q10" s="34" t="e">
-        <f ca="1">IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
-        <v>#NAME?</v>
+      <c r="Q10" s="34" t="str">
+        <f>IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
+        <v/>
       </c>
       <c r="R10" s="8" t="s">
         <v>13</v>
@@ -1876,20 +1894,20 @@
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>GBPSTD</v>
       </c>
-      <c r="L11" s="24" t="e">
-        <f ca="1">_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M11" s="25" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(K11,L11)</f>
-        <v>#NAME?</v>
+      <c r="L11" s="24">
+        <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
+        <v>41983</v>
+      </c>
+      <c r="M11" s="25">
+        <f>_xll.qlYieldTSDiscount(K11,L11)</f>
+        <v>1</v>
       </c>
       <c r="N11" s="25"/>
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
-      <c r="Q11" s="35" t="e">
-        <f ca="1">IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
-        <v>#NAME?</v>
+      <c r="Q11" s="35" t="str">
+        <f>IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
+        <v/>
       </c>
       <c r="R11" s="8" t="s">
         <v>13</v>
@@ -1938,20 +1956,20 @@
         <f>UPPER(Currency)&amp;"ON"</f>
         <v>GBPON</v>
       </c>
-      <c r="L12" s="24" t="e">
-        <f ca="1">_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M12" s="25" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(K12,L12)</f>
-        <v>#NAME?</v>
+      <c r="L12" s="24">
+        <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
+        <v>41983</v>
+      </c>
+      <c r="M12" s="25">
+        <f>_xll.qlYieldTSDiscount(K12,L12)</f>
+        <v>1</v>
       </c>
       <c r="N12" s="25"/>
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
-      <c r="Q12" s="35" t="e">
-        <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
-        <v>#NAME?</v>
+      <c r="Q12" s="35" t="str">
+        <f>IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
+        <v/>
       </c>
       <c r="R12" s="8" t="s">
         <v>13</v>
@@ -1990,20 +2008,20 @@
         <f>UPPER(Currency)&amp;"1M"</f>
         <v>GBP1M</v>
       </c>
-      <c r="L13" s="24" t="e">
-        <f ca="1">_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M13" s="25" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(K13,L13)</f>
-        <v>#NAME?</v>
+      <c r="L13" s="24">
+        <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
+        <v>41983</v>
+      </c>
+      <c r="M13" s="25">
+        <f>_xll.qlYieldTSDiscount(K13,L13)</f>
+        <v>1</v>
       </c>
       <c r="N13" s="25"/>
       <c r="O13" s="25"/>
       <c r="P13" s="25"/>
-      <c r="Q13" s="36" t="e">
-        <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
-        <v>#NAME?</v>
+      <c r="Q13" s="36" t="str">
+        <f>IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
+        <v/>
       </c>
       <c r="R13" s="8" t="s">
         <v>13</v>
@@ -2032,13 +2050,13 @@
       <c r="B14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C14" s="37" t="e">
-        <f t="array" aca="1" ref="C14:C17" ca="1">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D14" s="6" t="e">
-        <f t="array" aca="1" ref="D14:D17" ca="1">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
-        <v>#NAME?</v>
+      <c r="C14" s="37">
+        <f t="array" ref="C14:C17">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
+        <v>41990</v>
+      </c>
+      <c r="D14" s="6" t="str">
+        <f t="array" ref="D14:D17">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
+        <v>FSSZ4</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -2050,20 +2068,20 @@
         <f>UPPER(Currency)&amp;"3M"</f>
         <v>GBP3M</v>
       </c>
-      <c r="L14" s="24" t="e">
-        <f ca="1">_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M14" s="25" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(K14,L14)</f>
-        <v>#NAME?</v>
+      <c r="L14" s="24">
+        <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
+        <v>41983</v>
+      </c>
+      <c r="M14" s="25">
+        <f>_xll.qlYieldTSDiscount(K14,L14)</f>
+        <v>1</v>
       </c>
       <c r="N14" s="25"/>
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
-      <c r="Q14" s="36" t="e">
-        <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
-        <v>#NAME?</v>
+      <c r="Q14" s="36" t="str">
+        <f>IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
+        <v/>
       </c>
       <c r="R14" s="8" t="s">
         <v>13</v>
@@ -2092,13 +2110,11 @@
       <c r="B15" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="C15" s="38" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D15" s="8" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="C15" s="38">
+        <v>42081</v>
+      </c>
+      <c r="D15" s="8" t="str">
+        <v>FSSH5</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -2110,20 +2126,20 @@
         <f>UPPER(Currency)&amp;"6M"</f>
         <v>GBP6M</v>
       </c>
-      <c r="L15" s="24" t="e">
-        <f ca="1">_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M15" s="25" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(K15,L15)</f>
-        <v>#NAME?</v>
+      <c r="L15" s="24">
+        <f>_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
+        <v>41983</v>
+      </c>
+      <c r="M15" s="25">
+        <f>_xll.qlYieldTSDiscount(K15,L15)</f>
+        <v>1</v>
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="25"/>
       <c r="P15" s="25"/>
-      <c r="Q15" s="36" t="e">
-        <f ca="1">IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
-        <v>#NAME?</v>
+      <c r="Q15" s="36" t="str">
+        <f>IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
+        <v/>
       </c>
       <c r="R15" s="8" t="s">
         <v>13</v>
@@ -2152,13 +2168,11 @@
       <c r="B16" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="38" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D16" s="8" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="C16" s="38">
+        <v>42172</v>
+      </c>
+      <c r="D16" s="8" t="str">
+        <v>FSSM5</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2170,20 +2184,20 @@
         <f>UPPER(Currency)&amp;"1Y"</f>
         <v>GBP1Y</v>
       </c>
-      <c r="L16" s="44" t="e">
-        <f ca="1">_xll.qlTermStructureReferenceDate(K16,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M16" s="45" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(K16,L16)</f>
-        <v>#NAME?</v>
+      <c r="L16" s="44">
+        <f>_xll.qlTermStructureReferenceDate(K16,Trigger)</f>
+        <v>41983</v>
+      </c>
+      <c r="M16" s="45">
+        <f>_xll.qlYieldTSDiscount(K16,L16)</f>
+        <v>1</v>
       </c>
       <c r="N16" s="45"/>
       <c r="O16" s="45"/>
       <c r="P16" s="45"/>
-      <c r="Q16" s="46" t="e">
-        <f ca="1">IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
-        <v>#NAME?</v>
+      <c r="Q16" s="46" t="str">
+        <f>IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
+        <v/>
       </c>
       <c r="R16" s="8" t="s">
         <v>13</v>
@@ -2212,13 +2226,11 @@
       <c r="B17" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="C17" s="39" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D17" s="10" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="C17" s="39">
+        <v>42263</v>
+      </c>
+      <c r="D17" s="10" t="str">
+        <v>FSSU5</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -5439,7 +5451,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="CommandButton2">
+        <control shapeId="1025" r:id="rId4" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5459,12 +5471,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="CommandButton1">
+        <control shapeId="1026" r:id="rId6" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5484,7 +5496,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>